<commit_message>
Changed excel sheet to include colored cells for correct tests
</commit_message>
<xml_diff>
--- a/ClueGameBoard.xlsx
+++ b/ClueGameBoard.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ConnorKoch\Downloads\ClueBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ConnorKoch\eclipse-workspace\C12A-Clue\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26190" windowHeight="9420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="31">
   <si>
     <t>A</t>
   </si>
@@ -96,6 +96,27 @@
   </si>
   <si>
     <t>CR</t>
+  </si>
+  <si>
+    <t>Number of doors:  16</t>
+  </si>
+  <si>
+    <t>White: door direction tests</t>
+  </si>
+  <si>
+    <t>Orange: adj list tests, inside room</t>
+  </si>
+  <si>
+    <t>Purple: adj list tests, room exits</t>
+  </si>
+  <si>
+    <t>Green: adj lists beside room entrance</t>
+  </si>
+  <si>
+    <t>Light Blue: test targets</t>
+  </si>
+  <si>
+    <t>Light Green: walkway scenarios</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,6 +163,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -155,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,12 +223,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCECFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -452,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z26"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +547,7 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -541,7 +612,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -737,7 +808,7 @@
       <c r="L4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="2" t="s">
@@ -850,7 +921,7 @@
       <c r="W5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="9" t="s">
         <v>5</v>
       </c>
       <c r="Y5" s="1" t="s">
@@ -885,7 +956,7 @@
       <c r="H6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="6" t="s">
         <v>20</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -965,7 +1036,7 @@
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -1173,7 +1244,7 @@
       <c r="X9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Y9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="Z9" s="3">
@@ -1430,7 +1501,7 @@
       <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -1504,7 +1575,7 @@
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1516,10 +1587,10 @@
       <c r="E14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1650,7 +1721,7 @@
       <c r="W15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="X15" s="4" t="s">
+      <c r="X15" s="6" t="s">
         <v>17</v>
       </c>
       <c r="Y15" s="1" t="s">
@@ -1993,7 +2064,7 @@
       <c r="D20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -2023,7 +2094,7 @@
       <c r="N20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O20" s="2" t="s">
+      <c r="O20" s="4" t="s">
         <v>1</v>
       </c>
       <c r="P20" s="2" t="s">
@@ -2141,7 +2212,7 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2364,7 +2435,7 @@
       <c r="U24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="V24" s="2" t="s">
+      <c r="V24" s="7" t="s">
         <v>1</v>
       </c>
       <c r="W24" s="4" t="s">
@@ -2396,7 +2467,7 @@
       <c r="E25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2537,6 +2608,41 @@
         <v>24</v>
       </c>
       <c r="Z26" s="3"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>